<commit_message>
Fix trading notebook and smile notebook, add new trades, reorganize folders
</commit_message>
<xml_diff>
--- a/data/IV smile data.xlsx
+++ b/data/IV smile data.xlsx
@@ -7,10 +7,10 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="20161014 SPY IV smile data" sheetId="1" r:id="rId1"/>
+    <sheet name="20161014 EWZ IV smile data" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_20160928_UNG" localSheetId="0">'20161014 SPY IV smile data'!$A$1:$D$52</definedName>
+    <definedName name="_20160928_UNG" localSheetId="0">'20161014 EWZ IV smile data'!$A$1:$D$53</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
@@ -30,11 +30,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>option_type</t>
   </si>
   <si>
+    <t>strike_buy</t>
+  </si>
+  <si>
     <t>ticker</t>
   </si>
   <si>
@@ -47,6 +50,9 @@
     <t>expiration_dd</t>
   </si>
   <si>
+    <t>strike_write</t>
+  </si>
+  <si>
     <t>FIELD</t>
   </si>
   <si>
@@ -62,25 +68,52 @@
     <t>put</t>
   </si>
   <si>
-    <t>SPY</t>
-  </si>
-  <si>
     <t>E:\\Datos\\bolsa\\cuenta personal\\analisis de valores\\Trades activos\\Scanning\\20161014</t>
   </si>
   <si>
-    <t>20161014 SPY</t>
-  </si>
-  <si>
-    <t>entry_date_yy</t>
-  </si>
-  <si>
-    <t>entry_date_mm</t>
-  </si>
-  <si>
-    <t>entry_date_dd</t>
-  </si>
-  <si>
     <t>historical_volatility</t>
+  </si>
+  <si>
+    <t>entry_date_hh_buy</t>
+  </si>
+  <si>
+    <t>entry_date_MM_buy</t>
+  </si>
+  <si>
+    <t>entry_date_ss_buy</t>
+  </si>
+  <si>
+    <t>entry_date_yy_buy</t>
+  </si>
+  <si>
+    <t>entry_date_mm_buy</t>
+  </si>
+  <si>
+    <t>entry_date_dd_buy</t>
+  </si>
+  <si>
+    <t>entry_date_yy_write</t>
+  </si>
+  <si>
+    <t>entry_date_mm_write</t>
+  </si>
+  <si>
+    <t>entry_date_dd_write</t>
+  </si>
+  <si>
+    <t>entry_date_hh_write</t>
+  </si>
+  <si>
+    <t>entry_date_MM_write</t>
+  </si>
+  <si>
+    <t>entry_date_ss_write</t>
+  </si>
+  <si>
+    <t>20161014 EWZ</t>
+  </si>
+  <si>
+    <t>EWZ</t>
   </si>
 </sst>
 </file>
@@ -456,10 +489,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -473,28 +506,28 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -502,15 +535,15 @@
         <v>0</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="4">
-        <v>2016</v>
+      <c r="B5" s="4" t="s">
+        <v>27</v>
       </c>
       <c r="F5" s="2"/>
     </row>
@@ -519,7 +552,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="4">
-        <v>10</v>
+        <v>2016</v>
       </c>
       <c r="F6" s="2"/>
     </row>
@@ -528,66 +561,147 @@
         <v>4</v>
       </c>
       <c r="B7" s="4">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="F7" s="2"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B8" s="4">
-        <v>2016</v>
+        <v>21</v>
       </c>
       <c r="F8" s="2"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="B9" s="4">
-        <v>10</v>
-      </c>
-      <c r="F9" s="1"/>
+        <v>35</v>
+      </c>
+      <c r="F9" s="2"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B10" s="4">
-        <v>14</v>
-      </c>
-      <c r="F10" s="2"/>
+        <v>2016</v>
+      </c>
+      <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="4">
         <v>10</v>
       </c>
       <c r="F11" s="2"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="4">
+        <v>14</v>
+      </c>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="4">
+        <v>9</v>
+      </c>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="4">
+        <v>50</v>
+      </c>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B15" s="4">
+        <v>23</v>
+      </c>
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="4">
+        <v>36</v>
+      </c>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="4">
+        <v>2016</v>
+      </c>
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="4">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="4">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="4">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="4">
         <v>0</v>
       </c>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F15" s="2"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F16" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>